<commit_message>
commit 14 de febrero
</commit_message>
<xml_diff>
--- a/BD paper/catalogos/waveform_3p1_filtered.xlsx
+++ b/BD paper/catalogos/waveform_3p1_filtered.xlsx
@@ -495,37 +495,37 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Estación más cercana 6</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Estación más cercana 7</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Inicio estación más cercana 1</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Inicio estación más cercana 2</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Inicio estación más cercana 3</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Inicio estación más cercana 4</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Inicio estación más cercana 5</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Estación más cercana 6</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Estación más cercana 7</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
@@ -587,37 +587,37 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>PB10</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>2014-07-26T21:25:18</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>2014-07-26T21:25:20</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>2014-07-26T21:25:20</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>2014-07-26T21:25:23</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>2014-07-26T21:25:25</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>PB03</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>PB10</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -679,37 +679,37 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
           <t>2014-06-28T15:47:42</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>2014-06-28T15:47:43</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>2014-06-28T15:47:46</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>2014-06-28T15:47:47</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>2014-06-28T15:47:48</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>PATCX</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -771,37 +771,37 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>PB05</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
           <t>2014-07-13T19:00:28</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>2014-07-13T19:00:34</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>2014-07-13T19:00:35</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>2014-07-13T19:00:37</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>2014-07-13T19:00:38</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>PB15</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>PB05</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -863,37 +863,37 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
           <t>2014-10-19T08:02:35</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>2014-10-19T08:02:35</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>2014-10-19T08:02:37</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>2014-10-19T08:02:39</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>2014-10-19T08:02:40</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>TA01</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>HMBCX</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
@@ -955,37 +955,37 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>CO04</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
           <t>2015-03-13T00:22:05</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>2015-03-13T00:22:06</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>2015-03-13T00:22:08</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>2015-03-13T00:22:09</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>2015-03-13T00:22:09</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>MT02</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>CO04</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1047,37 +1047,37 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
+          <t>CO05</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>GO04</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
           <t>2015-04-13T23:36:39</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>2015-04-13T23:36:46</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>2015-04-13T23:36:48</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>2015-04-13T23:36:49</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>2015-04-13T23:36:49</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>CO05</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>GO04</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -1139,37 +1139,37 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
+          <t>AC05</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
           <t>2015-04-29T11:34:20</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>2015-04-29T11:34:25</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>2015-04-29T11:34:26</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>2015-04-29T11:34:27</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>2015-04-29T11:34:27</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>AC05</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>CO10</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -1231,37 +1231,37 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
+          <t>ME06</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>MT07</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
           <t>2015-08-12T17:45:33</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>2015-08-12T17:45:37</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>2015-08-12T17:45:38</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>2015-08-12T17:45:38</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>2015-08-12T17:45:38</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>ME06</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>MT07</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -1323,37 +1323,37 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
           <t>2015-08-27T18:15:06</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>2015-08-27T18:15:07</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>2015-08-27T18:15:11</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>2015-08-27T18:15:17</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>2015-08-27T18:15:18</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>PSGCX</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>MNMCX</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
@@ -1415,37 +1415,37 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
+          <t>MT07</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
           <t>2015-09-18T21:26:20</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>2015-09-18T21:26:23</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>2015-09-18T21:26:24</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>2015-09-18T21:26:25</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>2015-09-18T21:26:26</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>MT07</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>MT02</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -1507,37 +1507,37 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
+          <t>MT07</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
           <t>2015-09-19T13:36:00</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>2015-09-19T13:36:02</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>2015-09-19T13:36:05</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>2015-09-19T13:36:05</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>2015-09-19T13:36:06</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>MT07</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>MT02</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -1599,37 +1599,37 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
+          <t>CO04</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
           <t>2016-05-01T01:15:49</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>2016-05-01T01:15:49</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>2016-05-01T01:15:51</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>2016-05-01T01:15:53</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="R13" t="inlineStr">
         <is>
           <t>2016-05-01T01:15:53</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>CO04</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>MT02</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -1691,37 +1691,37 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
           <t>2014-01-04T08:25:43</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>2014-01-04T08:25:43</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>2014-01-04T08:25:45</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>2014-01-04T08:25:47</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>2014-01-04T08:25:49</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -1783,37 +1783,37 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
           <t>2014-01-04T18:56:36</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>2014-01-04T18:56:39</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>2014-01-04T18:56:41</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>2014-01-04T18:56:42</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>2014-01-04T18:56:44</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>PX05</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>PB03</t>
         </is>
       </c>
       <c r="S15" t="inlineStr">
@@ -1875,37 +1875,37 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
           <t>2014-01-06T12:14:11</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>2014-01-06T12:14:11</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>2014-01-06T12:14:13</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>2014-01-06T12:14:15</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>2014-01-06T12:14:18</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
@@ -1967,37 +1967,37 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
           <t>2014-01-06T15:01:24</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="O17" t="inlineStr">
         <is>
           <t>2014-01-06T15:01:24</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr">
+      <c r="P17" t="inlineStr">
         <is>
           <t>2014-01-06T15:01:26</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="Q17" t="inlineStr">
         <is>
           <t>2014-01-06T15:01:29</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="R17" t="inlineStr">
         <is>
           <t>2014-01-06T15:01:31</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
@@ -2059,37 +2059,37 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
           <t>2014-01-08T18:11:55</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>2014-01-08T18:11:55</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>2014-01-08T18:11:57</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>2014-01-08T18:12:00</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="R18" t="inlineStr">
         <is>
           <t>2014-01-08T18:12:02</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
@@ -2151,37 +2151,37 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
           <t>2014-01-08T20:35:42</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="O19" t="inlineStr">
         <is>
           <t>2014-01-08T20:35:42</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>2014-01-08T20:35:45</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="Q19" t="inlineStr">
         <is>
           <t>2014-01-08T20:35:47</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="R19" t="inlineStr">
         <is>
           <t>2014-01-08T20:35:49</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
@@ -2243,37 +2243,37 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
           <t>2014-01-11T13:43:32</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>2014-01-11T13:43:33</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>2014-01-11T13:43:35</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
         <is>
           <t>2014-01-11T13:43:37</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
+      <c r="R20" t="inlineStr">
         <is>
           <t>2014-01-11T13:43:39</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
@@ -2335,37 +2335,37 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
+          <t>AC05</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
           <t>2014-01-14T10:30:37</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="O21" t="inlineStr">
         <is>
           <t>2014-01-14T10:30:42</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>2014-01-14T10:30:42</t>
         </is>
       </c>
-      <c r="O21" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>2014-01-14T10:30:43</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="R21" t="inlineStr">
         <is>
           <t>2014-01-14T10:30:43</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>AC05</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>CO10</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
@@ -2427,37 +2427,37 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
           <t>2014-01-18T15:49:55</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="O22" t="inlineStr">
         <is>
           <t>2014-01-18T15:49:57</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr">
+      <c r="P22" t="inlineStr">
         <is>
           <t>2014-01-18T15:49:59</t>
         </is>
       </c>
-      <c r="O22" t="inlineStr">
+      <c r="Q22" t="inlineStr">
         <is>
           <t>2014-01-18T15:50:01</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
+      <c r="R22" t="inlineStr">
         <is>
           <t>2014-01-18T15:50:02</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>PSGCX</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
@@ -2519,37 +2519,37 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
           <t>2014-01-22T17:36:54</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="O23" t="inlineStr">
         <is>
           <t>2014-01-22T17:36:54</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr">
+      <c r="P23" t="inlineStr">
         <is>
           <t>2014-01-22T17:36:57</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
+      <c r="Q23" t="inlineStr">
         <is>
           <t>2014-01-22T17:36:59</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
+      <c r="R23" t="inlineStr">
         <is>
           <t>2014-01-22T17:37:01</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S23" t="inlineStr">
@@ -2611,37 +2611,37 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
           <t>2014-02-24T23:30:40</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="O24" t="inlineStr">
         <is>
           <t>2014-02-24T23:30:43</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr">
+      <c r="P24" t="inlineStr">
         <is>
           <t>2014-02-24T23:30:46</t>
         </is>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="Q24" t="inlineStr">
         <is>
           <t>2014-02-24T23:30:47</t>
         </is>
       </c>
-      <c r="P24" t="inlineStr">
+      <c r="R24" t="inlineStr">
         <is>
           <t>2014-02-24T23:30:47</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>PB12</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>HMBCX</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
@@ -2703,37 +2703,37 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
+          <t>PB10</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
           <t>2014-03-10T08:59:33</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="O25" t="inlineStr">
         <is>
           <t>2014-03-10T08:59:35</t>
         </is>
       </c>
-      <c r="N25" t="inlineStr">
+      <c r="P25" t="inlineStr">
         <is>
           <t>2014-03-10T08:59:36</t>
         </is>
       </c>
-      <c r="O25" t="inlineStr">
+      <c r="Q25" t="inlineStr">
         <is>
           <t>2014-03-10T08:59:39</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr">
+      <c r="R25" t="inlineStr">
         <is>
           <t>2014-03-10T08:59:40</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>PB10</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>PB06</t>
         </is>
       </c>
       <c r="S25" t="inlineStr">
@@ -2795,37 +2795,37 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
           <t>2014-03-13T03:32:23</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="O26" t="inlineStr">
         <is>
           <t>2014-03-13T03:32:25</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr">
+      <c r="P26" t="inlineStr">
         <is>
           <t>2014-03-13T03:32:26</t>
         </is>
       </c>
-      <c r="O26" t="inlineStr">
+      <c r="Q26" t="inlineStr">
         <is>
           <t>2014-03-13T03:32:29</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr">
+      <c r="R26" t="inlineStr">
         <is>
           <t>2014-03-13T03:32:29</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>PB03</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>PX05</t>
         </is>
       </c>
       <c r="S26" t="inlineStr">
@@ -2887,37 +2887,37 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
           <t>2014-03-15T02:47:09</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="O27" t="inlineStr">
         <is>
           <t>2014-03-15T02:47:10</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr">
+      <c r="P27" t="inlineStr">
         <is>
           <t>2014-03-15T02:47:11</t>
         </is>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="Q27" t="inlineStr">
         <is>
           <t>2014-03-15T02:47:13</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr">
+      <c r="R27" t="inlineStr">
         <is>
           <t>2014-03-15T02:47:13</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>PB02</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
@@ -2979,37 +2979,37 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
           <t>2014-03-18T16:46:27</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr">
+      <c r="O28" t="inlineStr">
         <is>
           <t>2014-03-18T16:46:28</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr">
+      <c r="P28" t="inlineStr">
         <is>
           <t>2014-03-18T16:46:29</t>
         </is>
       </c>
-      <c r="O28" t="inlineStr">
+      <c r="Q28" t="inlineStr">
         <is>
           <t>2014-03-18T16:46:30</t>
         </is>
       </c>
-      <c r="P28" t="inlineStr">
+      <c r="R28" t="inlineStr">
         <is>
           <t>2014-03-18T16:46:31</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S28" t="inlineStr">
@@ -3071,37 +3071,37 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
           <t>2014-03-19T12:23:23</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr">
+      <c r="O29" t="inlineStr">
         <is>
           <t>2014-03-19T12:23:25</t>
         </is>
       </c>
-      <c r="N29" t="inlineStr">
+      <c r="P29" t="inlineStr">
         <is>
           <t>2014-03-19T12:23:27</t>
         </is>
       </c>
-      <c r="O29" t="inlineStr">
+      <c r="Q29" t="inlineStr">
         <is>
           <t>2014-03-19T12:23:28</t>
         </is>
       </c>
-      <c r="P29" t="inlineStr">
+      <c r="R29" t="inlineStr">
         <is>
           <t>2014-03-19T12:23:28</t>
-        </is>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>PATCX</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
@@ -3163,37 +3163,37 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
           <t>2014-03-19T21:15:30</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="O30" t="inlineStr">
         <is>
           <t>2014-03-19T21:15:31</t>
         </is>
       </c>
-      <c r="N30" t="inlineStr">
+      <c r="P30" t="inlineStr">
         <is>
           <t>2014-03-19T21:15:32</t>
         </is>
       </c>
-      <c r="O30" t="inlineStr">
+      <c r="Q30" t="inlineStr">
         <is>
           <t>2014-03-19T21:15:33</t>
         </is>
       </c>
-      <c r="P30" t="inlineStr">
+      <c r="R30" t="inlineStr">
         <is>
           <t>2014-03-19T21:15:35</t>
-        </is>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
@@ -3255,37 +3255,37 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
           <t>2014-03-22T18:52:52</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr">
+      <c r="O31" t="inlineStr">
         <is>
           <t>2014-03-22T18:52:53</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr">
+      <c r="P31" t="inlineStr">
         <is>
           <t>2014-03-22T18:52:53</t>
         </is>
       </c>
-      <c r="O31" t="inlineStr">
+      <c r="Q31" t="inlineStr">
         <is>
           <t>2014-03-22T18:52:55</t>
         </is>
       </c>
-      <c r="P31" t="inlineStr">
+      <c r="R31" t="inlineStr">
         <is>
           <t>2014-03-22T18:52:56</t>
-        </is>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
@@ -3347,37 +3347,37 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
+          <t>AC02</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>GO02</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
           <t>2014-03-25T22:08:50</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr">
+      <c r="O32" t="inlineStr">
         <is>
           <t>2014-03-25T22:08:56</t>
         </is>
       </c>
-      <c r="N32" t="inlineStr">
+      <c r="P32" t="inlineStr">
         <is>
           <t>2014-03-25T22:08:57</t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="Q32" t="inlineStr">
         <is>
           <t>2014-03-25T22:09:00</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr">
+      <c r="R32" t="inlineStr">
         <is>
           <t>2014-03-25T22:09:04</t>
-        </is>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>AC02</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>GO02</t>
         </is>
       </c>
       <c r="S32" t="inlineStr">
@@ -3439,37 +3439,37 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>AP01</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
           <t>2014-03-26T15:01:14</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr">
+      <c r="O33" t="inlineStr">
         <is>
           <t>2014-03-26T15:01:17</t>
         </is>
       </c>
-      <c r="N33" t="inlineStr">
+      <c r="P33" t="inlineStr">
         <is>
           <t>2014-03-26T15:01:17</t>
         </is>
       </c>
-      <c r="O33" t="inlineStr">
+      <c r="Q33" t="inlineStr">
         <is>
           <t>2014-03-26T15:01:19</t>
         </is>
       </c>
-      <c r="P33" t="inlineStr">
+      <c r="R33" t="inlineStr">
         <is>
           <t>2014-03-26T15:01:19</t>
-        </is>
-      </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>HMBCX</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>AP01</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
@@ -3531,37 +3531,37 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
+          <t>MT07</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>VA06</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
           <t>2017-04-27T01:55:06</t>
         </is>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="O34" t="inlineStr">
         <is>
           <t>2017-04-27T01:55:06</t>
         </is>
       </c>
-      <c r="N34" t="inlineStr">
+      <c r="P34" t="inlineStr">
         <is>
           <t>2017-04-27T01:55:12</t>
         </is>
       </c>
-      <c r="O34" t="inlineStr">
+      <c r="Q34" t="inlineStr">
         <is>
           <t>2017-04-27T01:55:12</t>
         </is>
       </c>
-      <c r="P34" t="inlineStr">
+      <c r="R34" t="inlineStr">
         <is>
           <t>2017-04-27T01:55:13</t>
-        </is>
-      </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>MT07</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>VA06</t>
         </is>
       </c>
       <c r="S34" t="inlineStr">
@@ -3623,37 +3623,37 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
           <t>2014-04-01T18:57:48</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="O35" t="inlineStr">
         <is>
           <t>2014-04-01T18:57:50</t>
         </is>
       </c>
-      <c r="N35" t="inlineStr">
+      <c r="P35" t="inlineStr">
         <is>
           <t>2014-04-01T18:57:51</t>
         </is>
       </c>
-      <c r="O35" t="inlineStr">
+      <c r="Q35" t="inlineStr">
         <is>
           <t>2014-04-01T18:57:53</t>
         </is>
       </c>
-      <c r="P35" t="inlineStr">
+      <c r="R35" t="inlineStr">
         <is>
           <t>2014-04-01T18:57:53</t>
-        </is>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>PB12</t>
         </is>
       </c>
       <c r="S35" t="inlineStr">
@@ -3715,37 +3715,37 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
           <t>2014-04-02T04:57:51</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr">
+      <c r="O36" t="inlineStr">
         <is>
           <t>2014-04-02T04:57:51</t>
         </is>
       </c>
-      <c r="N36" t="inlineStr">
+      <c r="P36" t="inlineStr">
         <is>
           <t>2014-04-02T04:57:53</t>
         </is>
       </c>
-      <c r="O36" t="inlineStr">
+      <c r="Q36" t="inlineStr">
         <is>
           <t>2014-04-02T04:57:54</t>
         </is>
       </c>
-      <c r="P36" t="inlineStr">
+      <c r="R36" t="inlineStr">
         <is>
           <t>2014-04-02T04:57:56</t>
-        </is>
-      </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S36" t="inlineStr">
@@ -3807,37 +3807,37 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
           <t>2014-04-02T14:10:54</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr">
+      <c r="O37" t="inlineStr">
         <is>
           <t>2014-04-02T14:10:54</t>
         </is>
       </c>
-      <c r="N37" t="inlineStr">
+      <c r="P37" t="inlineStr">
         <is>
           <t>2014-04-02T14:10:56</t>
         </is>
       </c>
-      <c r="O37" t="inlineStr">
+      <c r="Q37" t="inlineStr">
         <is>
           <t>2014-04-02T14:10:59</t>
         </is>
       </c>
-      <c r="P37" t="inlineStr">
+      <c r="R37" t="inlineStr">
         <is>
           <t>2014-04-02T14:11:01</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S37" t="inlineStr">
@@ -3899,37 +3899,37 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
           <t>2014-04-04T07:13:24</t>
         </is>
       </c>
-      <c r="M38" t="inlineStr">
+      <c r="O38" t="inlineStr">
         <is>
           <t>2014-04-04T07:13:25</t>
         </is>
       </c>
-      <c r="N38" t="inlineStr">
+      <c r="P38" t="inlineStr">
         <is>
           <t>2014-04-04T07:13:27</t>
         </is>
       </c>
-      <c r="O38" t="inlineStr">
+      <c r="Q38" t="inlineStr">
         <is>
           <t>2014-04-04T07:13:28</t>
         </is>
       </c>
-      <c r="P38" t="inlineStr">
+      <c r="R38" t="inlineStr">
         <is>
           <t>2014-04-04T07:13:29</t>
-        </is>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>PATCX</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
@@ -3991,37 +3991,37 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
+          <t>AP01</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
           <t>2014-04-04T13:41:31</t>
         </is>
       </c>
-      <c r="M39" t="inlineStr">
+      <c r="O39" t="inlineStr">
         <is>
           <t>2014-04-04T13:41:31</t>
         </is>
       </c>
-      <c r="N39" t="inlineStr">
+      <c r="P39" t="inlineStr">
         <is>
           <t>2014-04-04T13:41:35</t>
         </is>
       </c>
-      <c r="O39" t="inlineStr">
+      <c r="Q39" t="inlineStr">
         <is>
           <t>2014-04-04T13:41:38</t>
         </is>
       </c>
-      <c r="P39" t="inlineStr">
+      <c r="R39" t="inlineStr">
         <is>
           <t>2014-04-04T13:41:40</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>AP01</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>PB12</t>
         </is>
       </c>
       <c r="S39" t="inlineStr">
@@ -4083,37 +4083,37 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
           <t>2014-04-05T12:23:16</t>
         </is>
       </c>
-      <c r="M40" t="inlineStr">
+      <c r="O40" t="inlineStr">
         <is>
           <t>2014-04-05T12:23:18</t>
         </is>
       </c>
-      <c r="N40" t="inlineStr">
+      <c r="P40" t="inlineStr">
         <is>
           <t>2014-04-05T12:23:18</t>
         </is>
       </c>
-      <c r="O40" t="inlineStr">
+      <c r="Q40" t="inlineStr">
         <is>
           <t>2014-04-05T12:23:19</t>
         </is>
       </c>
-      <c r="P40" t="inlineStr">
+      <c r="R40" t="inlineStr">
         <is>
           <t>2014-04-05T12:23:20</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>PX03</t>
         </is>
       </c>
       <c r="S40" t="inlineStr">
@@ -4175,37 +4175,37 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
           <t>2014-04-05T13:36:32</t>
         </is>
       </c>
-      <c r="M41" t="inlineStr">
+      <c r="O41" t="inlineStr">
         <is>
           <t>2014-04-05T13:36:33</t>
         </is>
       </c>
-      <c r="N41" t="inlineStr">
+      <c r="P41" t="inlineStr">
         <is>
           <t>2014-04-05T13:36:34</t>
         </is>
       </c>
-      <c r="O41" t="inlineStr">
+      <c r="Q41" t="inlineStr">
         <is>
           <t>2014-04-05T13:36:35</t>
         </is>
       </c>
-      <c r="P41" t="inlineStr">
+      <c r="R41" t="inlineStr">
         <is>
           <t>2014-04-05T13:36:36</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S41" t="inlineStr">
@@ -4267,37 +4267,37 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
           <t>2014-04-06T18:01:05</t>
         </is>
       </c>
-      <c r="M42" t="inlineStr">
+      <c r="O42" t="inlineStr">
         <is>
           <t>2014-04-06T18:01:06</t>
         </is>
       </c>
-      <c r="N42" t="inlineStr">
+      <c r="P42" t="inlineStr">
         <is>
           <t>2014-04-06T18:01:06</t>
         </is>
       </c>
-      <c r="O42" t="inlineStr">
+      <c r="Q42" t="inlineStr">
         <is>
           <t>2014-04-06T18:01:09</t>
         </is>
       </c>
-      <c r="P42" t="inlineStr">
+      <c r="R42" t="inlineStr">
         <is>
           <t>2014-04-06T18:01:12</t>
-        </is>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>PSGCX</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>PX03</t>
         </is>
       </c>
       <c r="S42" t="inlineStr">
@@ -4359,37 +4359,37 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
           <t>2014-04-06T19:42:32</t>
         </is>
       </c>
-      <c r="M43" t="inlineStr">
+      <c r="O43" t="inlineStr">
         <is>
           <t>2014-04-06T19:42:34</t>
         </is>
       </c>
-      <c r="N43" t="inlineStr">
+      <c r="P43" t="inlineStr">
         <is>
           <t>2014-04-06T19:42:36</t>
         </is>
       </c>
-      <c r="O43" t="inlineStr">
+      <c r="Q43" t="inlineStr">
         <is>
           <t>2014-04-06T19:42:36</t>
         </is>
       </c>
-      <c r="P43" t="inlineStr">
+      <c r="R43" t="inlineStr">
         <is>
           <t>2014-04-06T19:42:36</t>
-        </is>
-      </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>PATCX</t>
         </is>
       </c>
       <c r="S43" t="inlineStr">
@@ -4451,37 +4451,37 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
           <t>2014-04-07T19:54:39</t>
         </is>
       </c>
-      <c r="M44" t="inlineStr">
+      <c r="O44" t="inlineStr">
         <is>
           <t>2014-04-07T19:54:40</t>
         </is>
       </c>
-      <c r="N44" t="inlineStr">
+      <c r="P44" t="inlineStr">
         <is>
           <t>2014-04-07T19:54:41</t>
         </is>
       </c>
-      <c r="O44" t="inlineStr">
+      <c r="Q44" t="inlineStr">
         <is>
           <t>2014-04-07T19:54:42</t>
         </is>
       </c>
-      <c r="P44" t="inlineStr">
+      <c r="R44" t="inlineStr">
         <is>
           <t>2014-04-07T19:54:43</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>PX03</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
@@ -4543,37 +4543,37 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
           <t>2014-04-09T16:25:34</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr">
+      <c r="O45" t="inlineStr">
         <is>
           <t>2014-04-09T16:25:35</t>
         </is>
       </c>
-      <c r="N45" t="inlineStr">
+      <c r="P45" t="inlineStr">
         <is>
           <t>2014-04-09T16:25:35</t>
         </is>
       </c>
-      <c r="O45" t="inlineStr">
+      <c r="Q45" t="inlineStr">
         <is>
           <t>2014-04-09T16:25:37</t>
         </is>
       </c>
-      <c r="P45" t="inlineStr">
+      <c r="R45" t="inlineStr">
         <is>
           <t>2014-04-09T16:25:38</t>
-        </is>
-      </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S45" t="inlineStr">
@@ -4635,37 +4635,37 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
           <t>2014-04-13T13:28:21</t>
         </is>
       </c>
-      <c r="M46" t="inlineStr">
+      <c r="O46" t="inlineStr">
         <is>
           <t>2014-04-13T13:28:22</t>
         </is>
       </c>
-      <c r="N46" t="inlineStr">
+      <c r="P46" t="inlineStr">
         <is>
           <t>2014-04-13T13:28:23</t>
         </is>
       </c>
-      <c r="O46" t="inlineStr">
+      <c r="Q46" t="inlineStr">
         <is>
           <t>2014-04-13T13:28:25</t>
         </is>
       </c>
-      <c r="P46" t="inlineStr">
+      <c r="R46" t="inlineStr">
         <is>
           <t>2014-04-13T13:28:26</t>
-        </is>
-      </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S46" t="inlineStr">
@@ -4727,37 +4727,37 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
           <t>2014-04-26T20:37:03</t>
         </is>
       </c>
-      <c r="M47" t="inlineStr">
+      <c r="O47" t="inlineStr">
         <is>
           <t>2014-04-26T20:37:04</t>
         </is>
       </c>
-      <c r="N47" t="inlineStr">
+      <c r="P47" t="inlineStr">
         <is>
           <t>2014-04-26T20:37:07</t>
         </is>
       </c>
-      <c r="O47" t="inlineStr">
+      <c r="Q47" t="inlineStr">
         <is>
           <t>2014-04-26T20:37:07</t>
         </is>
       </c>
-      <c r="P47" t="inlineStr">
+      <c r="R47" t="inlineStr">
         <is>
           <t>2014-04-26T20:37:08</t>
-        </is>
-      </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>PATCX</t>
-        </is>
-      </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>PX02</t>
         </is>
       </c>
       <c r="S47" t="inlineStr">
@@ -4819,37 +4819,37 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
           <t>2014-04-28T11:03:56</t>
         </is>
       </c>
-      <c r="M48" t="inlineStr">
+      <c r="O48" t="inlineStr">
         <is>
           <t>2014-04-28T11:03:57</t>
         </is>
       </c>
-      <c r="N48" t="inlineStr">
+      <c r="P48" t="inlineStr">
         <is>
           <t>2014-04-28T11:03:57</t>
         </is>
       </c>
-      <c r="O48" t="inlineStr">
+      <c r="Q48" t="inlineStr">
         <is>
           <t>2014-04-28T11:04:00</t>
         </is>
       </c>
-      <c r="P48" t="inlineStr">
+      <c r="R48" t="inlineStr">
         <is>
           <t>2014-04-28T11:04:03</t>
-        </is>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>PB02</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
@@ -4911,37 +4911,37 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
+          <t>IN41</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>GO04</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
           <t>2014-04-29T04:06:34</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr">
+      <c r="O49" t="inlineStr">
         <is>
           <t>2014-04-29T04:06:40</t>
         </is>
       </c>
-      <c r="N49" t="inlineStr">
+      <c r="P49" t="inlineStr">
         <is>
           <t>2014-04-29T04:06:42</t>
         </is>
       </c>
-      <c r="O49" t="inlineStr">
+      <c r="Q49" t="inlineStr">
         <is>
           <t>2014-04-29T04:06:43</t>
         </is>
       </c>
-      <c r="P49" t="inlineStr">
+      <c r="R49" t="inlineStr">
         <is>
           <t>2014-04-29T04:06:43</t>
-        </is>
-      </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>IN41</t>
-        </is>
-      </c>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>GO04</t>
         </is>
       </c>
       <c r="S49" t="inlineStr">
@@ -5003,37 +5003,37 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
           <t>2014-04-30T09:39:51</t>
         </is>
       </c>
-      <c r="M50" t="inlineStr">
+      <c r="O50" t="inlineStr">
         <is>
           <t>2014-04-30T09:39:52</t>
         </is>
       </c>
-      <c r="N50" t="inlineStr">
+      <c r="P50" t="inlineStr">
         <is>
           <t>2014-04-30T09:39:54</t>
         </is>
       </c>
-      <c r="O50" t="inlineStr">
+      <c r="Q50" t="inlineStr">
         <is>
           <t>2014-04-30T09:39:55</t>
         </is>
       </c>
-      <c r="P50" t="inlineStr">
+      <c r="R50" t="inlineStr">
         <is>
           <t>2014-04-30T09:39:55</t>
-        </is>
-      </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>PATCX</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
@@ -5095,37 +5095,37 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
           <t>2014-04-30T14:39:09</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr">
+      <c r="O51" t="inlineStr">
         <is>
           <t>2014-04-30T14:39:10</t>
         </is>
       </c>
-      <c r="N51" t="inlineStr">
+      <c r="P51" t="inlineStr">
         <is>
           <t>2014-04-30T14:39:12</t>
         </is>
       </c>
-      <c r="O51" t="inlineStr">
+      <c r="Q51" t="inlineStr">
         <is>
           <t>2014-04-30T14:39:13</t>
         </is>
       </c>
-      <c r="P51" t="inlineStr">
+      <c r="R51" t="inlineStr">
         <is>
           <t>2014-04-30T14:39:14</t>
-        </is>
-      </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>PATCX</t>
-        </is>
-      </c>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>PB11</t>
         </is>
       </c>
       <c r="S51" t="inlineStr">
@@ -5187,37 +5187,37 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
           <t>2014-05-05T12:51:39</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr">
+      <c r="O52" t="inlineStr">
         <is>
           <t>2014-05-05T12:51:40</t>
         </is>
       </c>
-      <c r="N52" t="inlineStr">
+      <c r="P52" t="inlineStr">
         <is>
           <t>2014-05-05T12:51:40</t>
         </is>
       </c>
-      <c r="O52" t="inlineStr">
+      <c r="Q52" t="inlineStr">
         <is>
           <t>2014-05-05T12:51:43</t>
         </is>
       </c>
-      <c r="P52" t="inlineStr">
+      <c r="R52" t="inlineStr">
         <is>
           <t>2014-05-05T12:51:45</t>
-        </is>
-      </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>MNMCX</t>
-        </is>
-      </c>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>PB11</t>
         </is>
       </c>
       <c r="S52" t="inlineStr">
@@ -5279,37 +5279,37 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
+          <t>AC07</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
           <t>2014-05-10T16:40:25</t>
         </is>
       </c>
-      <c r="M53" t="inlineStr">
+      <c r="O53" t="inlineStr">
         <is>
           <t>2014-05-10T16:40:27</t>
         </is>
       </c>
-      <c r="N53" t="inlineStr">
+      <c r="P53" t="inlineStr">
         <is>
           <t>2014-05-10T16:40:28</t>
         </is>
       </c>
-      <c r="O53" t="inlineStr">
+      <c r="Q53" t="inlineStr">
         <is>
           <t>2014-05-10T16:40:29</t>
         </is>
       </c>
-      <c r="P53" t="inlineStr">
+      <c r="R53" t="inlineStr">
         <is>
           <t>2014-05-10T16:40:32</t>
-        </is>
-      </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>AC07</t>
-        </is>
-      </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>CO10</t>
         </is>
       </c>
       <c r="S53" t="inlineStr">
@@ -5371,37 +5371,37 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
+          <t>TLL</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>CO06</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
           <t>2014-05-15T17:45:47</t>
         </is>
       </c>
-      <c r="M54" t="inlineStr">
+      <c r="O54" t="inlineStr">
         <is>
           <t>2014-05-15T17:45:47</t>
         </is>
       </c>
-      <c r="N54" t="inlineStr">
+      <c r="P54" t="inlineStr">
         <is>
           <t>2014-05-15T17:45:48</t>
         </is>
       </c>
-      <c r="O54" t="inlineStr">
+      <c r="Q54" t="inlineStr">
         <is>
           <t>2014-05-15T17:45:53</t>
         </is>
       </c>
-      <c r="P54" t="inlineStr">
+      <c r="R54" t="inlineStr">
         <is>
           <t>2014-05-15T17:45:54</t>
-        </is>
-      </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>TLL</t>
-        </is>
-      </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>CO06</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
@@ -5463,37 +5463,37 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>TA02</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
           <t>2014-06-09T13:57:35</t>
         </is>
       </c>
-      <c r="M55" t="inlineStr">
+      <c r="O55" t="inlineStr">
         <is>
           <t>2014-06-09T13:57:35</t>
         </is>
       </c>
-      <c r="N55" t="inlineStr">
+      <c r="P55" t="inlineStr">
         <is>
           <t>2014-06-09T13:57:37</t>
         </is>
       </c>
-      <c r="O55" t="inlineStr">
+      <c r="Q55" t="inlineStr">
         <is>
           <t>2014-06-09T13:57:38</t>
         </is>
       </c>
-      <c r="P55" t="inlineStr">
+      <c r="R55" t="inlineStr">
         <is>
           <t>2014-06-09T13:57:38</t>
-        </is>
-      </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>PB01</t>
-        </is>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>TA02</t>
         </is>
       </c>
       <c r="S55" t="inlineStr">
@@ -5555,37 +5555,37 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
           <t>2014-06-10T06:14:36</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr">
+      <c r="O56" t="inlineStr">
         <is>
           <t>2014-06-10T06:14:37</t>
         </is>
       </c>
-      <c r="N56" t="inlineStr">
+      <c r="P56" t="inlineStr">
         <is>
           <t>2014-06-10T06:14:38</t>
         </is>
       </c>
-      <c r="O56" t="inlineStr">
+      <c r="Q56" t="inlineStr">
         <is>
           <t>2014-06-10T06:14:39</t>
         </is>
       </c>
-      <c r="P56" t="inlineStr">
+      <c r="R56" t="inlineStr">
         <is>
           <t>2014-06-10T06:14:40</t>
-        </is>
-      </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>PX02</t>
-        </is>
-      </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>PB11</t>
         </is>
       </c>
       <c r="S56" t="inlineStr">
@@ -5647,37 +5647,37 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
+          <t>TLL</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>CO03</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
           <t>2014-06-14T16:11:33</t>
         </is>
       </c>
-      <c r="M57" t="inlineStr">
+      <c r="O57" t="inlineStr">
         <is>
           <t>2014-06-14T16:11:34</t>
         </is>
       </c>
-      <c r="N57" t="inlineStr">
+      <c r="P57" t="inlineStr">
         <is>
           <t>2014-06-14T16:11:34</t>
         </is>
       </c>
-      <c r="O57" t="inlineStr">
+      <c r="Q57" t="inlineStr">
         <is>
           <t>2014-06-14T16:11:34</t>
         </is>
       </c>
-      <c r="P57" t="inlineStr">
+      <c r="R57" t="inlineStr">
         <is>
           <t>2014-06-14T16:11:37</t>
-        </is>
-      </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>TLL</t>
-        </is>
-      </c>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>CO03</t>
         </is>
       </c>
       <c r="S57" t="inlineStr">
@@ -5739,37 +5739,37 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
           <t>2014-08-27T18:13:42</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr">
+      <c r="O58" t="inlineStr">
         <is>
           <t>2014-08-27T18:13:47</t>
         </is>
       </c>
-      <c r="N58" t="inlineStr">
+      <c r="P58" t="inlineStr">
         <is>
           <t>2014-08-27T18:13:47</t>
         </is>
       </c>
-      <c r="O58" t="inlineStr">
+      <c r="Q58" t="inlineStr">
         <is>
           <t>2014-08-27T18:13:49</t>
         </is>
       </c>
-      <c r="P58" t="inlineStr">
+      <c r="R58" t="inlineStr">
         <is>
           <t>2014-08-27T18:13:50</t>
-        </is>
-      </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>TA01</t>
-        </is>
-      </c>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>MNMCX</t>
         </is>
       </c>
       <c r="S58" t="inlineStr">
@@ -5831,37 +5831,37 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
           <t>2014-09-01T20:41:37</t>
         </is>
       </c>
-      <c r="M59" t="inlineStr">
+      <c r="O59" t="inlineStr">
         <is>
           <t>2014-09-01T20:41:39</t>
         </is>
       </c>
-      <c r="N59" t="inlineStr">
+      <c r="P59" t="inlineStr">
         <is>
           <t>2014-09-01T20:41:40</t>
         </is>
       </c>
-      <c r="O59" t="inlineStr">
+      <c r="Q59" t="inlineStr">
         <is>
           <t>2014-09-01T20:41:40</t>
         </is>
       </c>
-      <c r="P59" t="inlineStr">
+      <c r="R59" t="inlineStr">
         <is>
           <t>2014-09-01T20:41:43</t>
-        </is>
-      </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>PB11</t>
-        </is>
-      </c>
-      <c r="R59" t="inlineStr">
-        <is>
-          <t>PX03</t>
         </is>
       </c>
       <c r="S59" t="inlineStr">
@@ -5923,37 +5923,37 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
+          <t>VA01</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>V25A</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
           <t>2014-09-12T16:14:35</t>
         </is>
       </c>
-      <c r="M60" t="inlineStr">
+      <c r="O60" t="inlineStr">
         <is>
           <t>2014-09-12T16:14:35</t>
         </is>
       </c>
-      <c r="N60" t="inlineStr">
+      <c r="P60" t="inlineStr">
         <is>
           <t>2014-09-12T16:14:36</t>
         </is>
       </c>
-      <c r="O60" t="inlineStr">
+      <c r="Q60" t="inlineStr">
         <is>
           <t>2014-09-12T16:14:39</t>
         </is>
       </c>
-      <c r="P60" t="inlineStr">
+      <c r="R60" t="inlineStr">
         <is>
           <t>2014-09-12T16:14:39</t>
-        </is>
-      </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>VA01</t>
-        </is>
-      </c>
-      <c r="R60" t="inlineStr">
-        <is>
-          <t>V25A</t>
         </is>
       </c>
       <c r="S60" t="inlineStr">
@@ -6015,37 +6015,37 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>TA02</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
           <t>2014-10-19T17:56:21</t>
         </is>
       </c>
-      <c r="M61" t="inlineStr">
+      <c r="O61" t="inlineStr">
         <is>
           <t>2014-10-19T17:56:23</t>
         </is>
       </c>
-      <c r="N61" t="inlineStr">
+      <c r="P61" t="inlineStr">
         <is>
           <t>2014-10-19T17:56:25</t>
         </is>
       </c>
-      <c r="O61" t="inlineStr">
+      <c r="Q61" t="inlineStr">
         <is>
           <t>2014-10-19T17:56:26</t>
         </is>
       </c>
-      <c r="P61" t="inlineStr">
+      <c r="R61" t="inlineStr">
         <is>
           <t>2014-10-19T17:56:26</t>
-        </is>
-      </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>PX05</t>
-        </is>
-      </c>
-      <c r="R61" t="inlineStr">
-        <is>
-          <t>TA02</t>
         </is>
       </c>
       <c r="S61" t="inlineStr">
@@ -6107,37 +6107,37 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
+          <t>AC05</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
           <t>2014-12-08T23:16:24</t>
         </is>
       </c>
-      <c r="M62" t="inlineStr">
+      <c r="O62" t="inlineStr">
         <is>
           <t>2014-12-08T23:16:34</t>
         </is>
       </c>
-      <c r="N62" t="inlineStr">
+      <c r="P62" t="inlineStr">
         <is>
           <t>2014-12-08T23:16:34</t>
         </is>
       </c>
-      <c r="O62" t="inlineStr">
+      <c r="Q62" t="inlineStr">
         <is>
           <t>2014-12-08T23:16:35</t>
         </is>
       </c>
-      <c r="P62" t="inlineStr">
+      <c r="R62" t="inlineStr">
         <is>
           <t>2014-12-08T23:16:35</t>
-        </is>
-      </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>AC05</t>
-        </is>
-      </c>
-      <c r="R62" t="inlineStr">
-        <is>
-          <t>CO10</t>
         </is>
       </c>
       <c r="S62" t="inlineStr">
@@ -6199,37 +6199,37 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>TA02</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
           <t>2015-01-02T01:02:21</t>
         </is>
       </c>
-      <c r="M63" t="inlineStr">
+      <c r="O63" t="inlineStr">
         <is>
           <t>2015-01-02T01:02:22</t>
         </is>
       </c>
-      <c r="N63" t="inlineStr">
+      <c r="P63" t="inlineStr">
         <is>
           <t>2015-01-02T01:02:23</t>
         </is>
       </c>
-      <c r="O63" t="inlineStr">
+      <c r="Q63" t="inlineStr">
         <is>
           <t>2015-01-02T01:02:26</t>
         </is>
       </c>
-      <c r="P63" t="inlineStr">
+      <c r="R63" t="inlineStr">
         <is>
           <t>2015-01-02T01:02:27</t>
-        </is>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>HMBCX</t>
-        </is>
-      </c>
-      <c r="R63" t="inlineStr">
-        <is>
-          <t>TA02</t>
         </is>
       </c>
       <c r="S63" t="inlineStr">
@@ -6291,37 +6291,37 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
+          <t>AC05</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
           <t>2015-01-21T17:52:05</t>
         </is>
       </c>
-      <c r="M64" t="inlineStr">
+      <c r="O64" t="inlineStr">
         <is>
           <t>2015-01-21T17:52:06</t>
         </is>
       </c>
-      <c r="N64" t="inlineStr">
+      <c r="P64" t="inlineStr">
         <is>
           <t>2015-01-21T17:52:06</t>
         </is>
       </c>
-      <c r="O64" t="inlineStr">
+      <c r="Q64" t="inlineStr">
         <is>
           <t>2015-01-21T17:52:07</t>
         </is>
       </c>
-      <c r="P64" t="inlineStr">
+      <c r="R64" t="inlineStr">
         <is>
           <t>2015-01-21T17:52:09</t>
-        </is>
-      </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>AC05</t>
-        </is>
-      </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>CO10</t>
         </is>
       </c>
       <c r="S64" t="inlineStr">
@@ -6383,37 +6383,37 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
+          <t>PB10</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>PB04</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
           <t>2015-03-09T06:17:19</t>
         </is>
       </c>
-      <c r="M65" t="inlineStr">
+      <c r="O65" t="inlineStr">
         <is>
           <t>2015-03-09T06:17:21</t>
         </is>
       </c>
-      <c r="N65" t="inlineStr">
+      <c r="P65" t="inlineStr">
         <is>
           <t>2015-03-09T06:17:23</t>
         </is>
       </c>
-      <c r="O65" t="inlineStr">
+      <c r="Q65" t="inlineStr">
         <is>
           <t>2015-03-09T06:17:24</t>
         </is>
       </c>
-      <c r="P65" t="inlineStr">
+      <c r="R65" t="inlineStr">
         <is>
           <t>2015-03-09T06:17:25</t>
-        </is>
-      </c>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>PB10</t>
-        </is>
-      </c>
-      <c r="R65" t="inlineStr">
-        <is>
-          <t>PB04</t>
         </is>
       </c>
       <c r="S65" t="inlineStr">
@@ -6475,37 +6475,37 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
           <t>2015-03-13T00:44:06</t>
         </is>
       </c>
-      <c r="M66" t="inlineStr">
+      <c r="O66" t="inlineStr">
         <is>
           <t>2015-03-13T00:44:10</t>
         </is>
       </c>
-      <c r="N66" t="inlineStr">
+      <c r="P66" t="inlineStr">
         <is>
           <t>2015-03-13T00:44:11</t>
         </is>
       </c>
-      <c r="O66" t="inlineStr">
+      <c r="Q66" t="inlineStr">
         <is>
           <t>2015-03-13T00:44:13</t>
         </is>
       </c>
-      <c r="P66" t="inlineStr">
+      <c r="R66" t="inlineStr">
         <is>
           <t>2015-03-13T00:44:13</t>
-        </is>
-      </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>PB15</t>
-        </is>
-      </c>
-      <c r="R66" t="inlineStr">
-        <is>
-          <t>PB03</t>
         </is>
       </c>
       <c r="S66" t="inlineStr">
@@ -6567,37 +6567,37 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
+          <t>IN41</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>GO04</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
           <t>2015-05-29T13:50:18</t>
         </is>
       </c>
-      <c r="M67" t="inlineStr">
+      <c r="O67" t="inlineStr">
         <is>
           <t>2015-05-29T13:50:24</t>
         </is>
       </c>
-      <c r="N67" t="inlineStr">
+      <c r="P67" t="inlineStr">
         <is>
           <t>2015-05-29T13:50:25</t>
         </is>
       </c>
-      <c r="O67" t="inlineStr">
+      <c r="Q67" t="inlineStr">
         <is>
           <t>2015-05-29T13:50:27</t>
         </is>
       </c>
-      <c r="P67" t="inlineStr">
+      <c r="R67" t="inlineStr">
         <is>
           <t>2015-05-29T13:50:27</t>
-        </is>
-      </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>IN41</t>
-        </is>
-      </c>
-      <c r="R67" t="inlineStr">
-        <is>
-          <t>GO04</t>
         </is>
       </c>
       <c r="S67" t="inlineStr">
@@ -6659,37 +6659,37 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
+          <t>CO05</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>CO03</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
           <t>2015-06-24T22:23:23</t>
         </is>
       </c>
-      <c r="M68" t="inlineStr">
+      <c r="O68" t="inlineStr">
         <is>
           <t>2015-06-24T22:23:23</t>
         </is>
       </c>
-      <c r="N68" t="inlineStr">
+      <c r="P68" t="inlineStr">
         <is>
           <t>2015-06-24T22:23:23</t>
         </is>
       </c>
-      <c r="O68" t="inlineStr">
+      <c r="Q68" t="inlineStr">
         <is>
           <t>2015-06-24T22:23:24</t>
         </is>
       </c>
-      <c r="P68" t="inlineStr">
+      <c r="R68" t="inlineStr">
         <is>
           <t>2015-06-24T22:23:24</t>
-        </is>
-      </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>CO05</t>
-        </is>
-      </c>
-      <c r="R68" t="inlineStr">
-        <is>
-          <t>CO03</t>
         </is>
       </c>
       <c r="S68" t="inlineStr">
@@ -6751,37 +6751,37 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
+          <t>PB13</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>PB16</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
           <t>2015-07-18T21:22:40</t>
         </is>
       </c>
-      <c r="M69" t="inlineStr">
+      <c r="O69" t="inlineStr">
         <is>
           <t>2015-07-18T21:22:41</t>
         </is>
       </c>
-      <c r="N69" t="inlineStr">
+      <c r="P69" t="inlineStr">
         <is>
           <t>2015-07-18T21:22:42</t>
         </is>
       </c>
-      <c r="O69" t="inlineStr">
+      <c r="Q69" t="inlineStr">
         <is>
           <t>2015-07-18T21:22:49</t>
         </is>
       </c>
-      <c r="P69" t="inlineStr">
+      <c r="R69" t="inlineStr">
         <is>
           <t>2015-07-18T21:22:50</t>
-        </is>
-      </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>PB13</t>
-        </is>
-      </c>
-      <c r="R69" t="inlineStr">
-        <is>
-          <t>PB16</t>
         </is>
       </c>
       <c r="S69" t="inlineStr">
@@ -6843,37 +6843,37 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
+          <t>VA01</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>ROC1</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
           <t>2015-07-19T09:18:31</t>
         </is>
       </c>
-      <c r="M70" t="inlineStr">
+      <c r="O70" t="inlineStr">
         <is>
           <t>2015-07-19T09:18:32</t>
         </is>
       </c>
-      <c r="N70" t="inlineStr">
+      <c r="P70" t="inlineStr">
         <is>
           <t>2015-07-19T09:18:33</t>
         </is>
       </c>
-      <c r="O70" t="inlineStr">
+      <c r="Q70" t="inlineStr">
         <is>
           <t>2015-07-19T09:18:35</t>
         </is>
       </c>
-      <c r="P70" t="inlineStr">
+      <c r="R70" t="inlineStr">
         <is>
           <t>2015-07-19T09:18:38</t>
-        </is>
-      </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>VA01</t>
-        </is>
-      </c>
-      <c r="R70" t="inlineStr">
-        <is>
-          <t>ROC1</t>
         </is>
       </c>
       <c r="S70" t="inlineStr">
@@ -6935,37 +6935,37 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
+          <t>IN41</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>GO04</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
           <t>2015-08-01T10:19:09</t>
         </is>
       </c>
-      <c r="M71" t="inlineStr">
+      <c r="O71" t="inlineStr">
         <is>
           <t>2015-08-01T10:19:17</t>
         </is>
       </c>
-      <c r="N71" t="inlineStr">
+      <c r="P71" t="inlineStr">
         <is>
           <t>2015-08-01T10:19:19</t>
         </is>
       </c>
-      <c r="O71" t="inlineStr">
+      <c r="Q71" t="inlineStr">
         <is>
           <t>2015-08-01T10:19:19</t>
         </is>
       </c>
-      <c r="P71" t="inlineStr">
+      <c r="R71" t="inlineStr">
         <is>
           <t>2015-08-01T10:19:19</t>
-        </is>
-      </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>IN41</t>
-        </is>
-      </c>
-      <c r="R71" t="inlineStr">
-        <is>
-          <t>GO04</t>
         </is>
       </c>
       <c r="S71" t="inlineStr">
@@ -7027,37 +7027,37 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>CO06</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
           <t>2015-08-23T23:26:08</t>
         </is>
       </c>
-      <c r="M72" t="inlineStr">
+      <c r="O72" t="inlineStr">
         <is>
           <t>2015-08-23T23:26:09</t>
         </is>
       </c>
-      <c r="N72" t="inlineStr">
+      <c r="P72" t="inlineStr">
         <is>
           <t>2015-08-23T23:26:09</t>
         </is>
       </c>
-      <c r="O72" t="inlineStr">
+      <c r="Q72" t="inlineStr">
         <is>
           <t>2015-08-23T23:26:14</t>
         </is>
       </c>
-      <c r="P72" t="inlineStr">
+      <c r="R72" t="inlineStr">
         <is>
           <t>2015-08-23T23:26:14</t>
-        </is>
-      </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>CO10</t>
-        </is>
-      </c>
-      <c r="R72" t="inlineStr">
-        <is>
-          <t>CO06</t>
         </is>
       </c>
       <c r="S72" t="inlineStr">
@@ -7119,37 +7119,37 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>CO06</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
           <t>2015-08-24T04:13:27</t>
         </is>
       </c>
-      <c r="M73" t="inlineStr">
+      <c r="O73" t="inlineStr">
         <is>
           <t>2015-08-24T04:13:28</t>
         </is>
       </c>
-      <c r="N73" t="inlineStr">
+      <c r="P73" t="inlineStr">
         <is>
           <t>2015-08-24T04:13:28</t>
         </is>
       </c>
-      <c r="O73" t="inlineStr">
+      <c r="Q73" t="inlineStr">
         <is>
           <t>2015-08-24T04:13:33</t>
         </is>
       </c>
-      <c r="P73" t="inlineStr">
+      <c r="R73" t="inlineStr">
         <is>
           <t>2015-08-24T04:13:33</t>
-        </is>
-      </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>CO10</t>
-        </is>
-      </c>
-      <c r="R73" t="inlineStr">
-        <is>
-          <t>CO06</t>
         </is>
       </c>
       <c r="S73" t="inlineStr">
@@ -7211,37 +7211,37 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
+          <t>TLL</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>CO06</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
           <t>2015-08-24T23:56:40</t>
         </is>
       </c>
-      <c r="M74" t="inlineStr">
+      <c r="O74" t="inlineStr">
         <is>
           <t>2015-08-24T23:56:41</t>
         </is>
       </c>
-      <c r="N74" t="inlineStr">
+      <c r="P74" t="inlineStr">
         <is>
           <t>2015-08-24T23:56:41</t>
         </is>
       </c>
-      <c r="O74" t="inlineStr">
+      <c r="Q74" t="inlineStr">
         <is>
           <t>2015-08-24T23:56:45</t>
         </is>
       </c>
-      <c r="P74" t="inlineStr">
+      <c r="R74" t="inlineStr">
         <is>
           <t>2015-08-24T23:56:46</t>
-        </is>
-      </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>TLL</t>
-        </is>
-      </c>
-      <c r="R74" t="inlineStr">
-        <is>
-          <t>CO06</t>
         </is>
       </c>
       <c r="S74" t="inlineStr">
@@ -7303,37 +7303,37 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
+          <t>V25A</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
           <t>2020-06-23T20:19:24</t>
         </is>
       </c>
-      <c r="M75" t="inlineStr">
+      <c r="O75" t="inlineStr">
         <is>
           <t>2020-06-23T20:19:27</t>
         </is>
       </c>
-      <c r="N75" t="inlineStr">
+      <c r="P75" t="inlineStr">
         <is>
           <t>2020-06-23T20:19:28</t>
         </is>
       </c>
-      <c r="O75" t="inlineStr">
+      <c r="Q75" t="inlineStr">
         <is>
           <t>2020-06-23T20:19:30</t>
         </is>
       </c>
-      <c r="P75" t="inlineStr">
+      <c r="R75" t="inlineStr">
         <is>
           <t>2020-06-23T20:19:30</t>
-        </is>
-      </c>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>V25A</t>
-        </is>
-      </c>
-      <c r="R75" t="inlineStr">
-        <is>
-          <t>MT02</t>
         </is>
       </c>
       <c r="S75" t="inlineStr">
@@ -7395,37 +7395,37 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
           <t>2020-10-06T11:32:48</t>
         </is>
       </c>
-      <c r="M76" t="inlineStr">
+      <c r="O76" t="inlineStr">
         <is>
           <t>2020-10-06T11:32:50</t>
         </is>
       </c>
-      <c r="N76" t="inlineStr">
+      <c r="P76" t="inlineStr">
         <is>
           <t>2020-10-06T11:32:55</t>
         </is>
       </c>
-      <c r="O76" t="inlineStr">
+      <c r="Q76" t="inlineStr">
         <is>
           <t>2020-10-06T11:32:55</t>
         </is>
       </c>
-      <c r="P76" t="inlineStr">
+      <c r="R76" t="inlineStr">
         <is>
           <t>2020-10-06T11:32:56</t>
-        </is>
-      </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>PX03</t>
-        </is>
-      </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>PB01</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -7487,37 +7487,37 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
+          <t>AP01</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>GO01</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
           <t>2020-10-11T07:06:17</t>
         </is>
       </c>
-      <c r="M77" t="inlineStr">
+      <c r="O77" t="inlineStr">
         <is>
           <t>2020-10-11T07:06:17</t>
         </is>
       </c>
-      <c r="N77" t="inlineStr">
+      <c r="P77" t="inlineStr">
         <is>
           <t>2020-10-11T07:06:20</t>
         </is>
       </c>
-      <c r="O77" t="inlineStr">
+      <c r="Q77" t="inlineStr">
         <is>
           <t>2020-10-11T07:06:22</t>
         </is>
       </c>
-      <c r="P77" t="inlineStr">
+      <c r="R77" t="inlineStr">
         <is>
           <t>2020-10-11T07:06:22</t>
-        </is>
-      </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>AP01</t>
-        </is>
-      </c>
-      <c r="R77" t="inlineStr">
-        <is>
-          <t>GO01</t>
         </is>
       </c>
       <c r="S77" t="inlineStr">
@@ -7579,37 +7579,37 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
+          <t>CO10</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>CO01</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
           <t>2020-11-18T05:31:40</t>
         </is>
       </c>
-      <c r="M78" t="inlineStr">
+      <c r="O78" t="inlineStr">
         <is>
           <t>2020-11-18T05:31:41</t>
         </is>
       </c>
-      <c r="N78" t="inlineStr">
+      <c r="P78" t="inlineStr">
         <is>
           <t>2020-11-18T05:31:42</t>
         </is>
       </c>
-      <c r="O78" t="inlineStr">
+      <c r="Q78" t="inlineStr">
         <is>
           <t>2020-11-18T05:31:44</t>
         </is>
       </c>
-      <c r="P78" t="inlineStr">
+      <c r="R78" t="inlineStr">
         <is>
           <t>2020-11-18T05:31:44</t>
-        </is>
-      </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>CO10</t>
-        </is>
-      </c>
-      <c r="R78" t="inlineStr">
-        <is>
-          <t>CO01</t>
         </is>
       </c>
       <c r="S78" t="inlineStr">

</xml_diff>